<commit_message>
Pushing final changes for hf challenge
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\qa-test-hf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C126F1-82DE-42C5-968C-6E7713B148A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FF52AF-1408-431B-A536-83ECF82294AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -956,10 +956,13 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="14.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>